<commit_message>
feat: update layout and data render
</commit_message>
<xml_diff>
--- a/dashboard-data.xlsx
+++ b/dashboard-data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
   <si>
     <t>project 1</t>
   </si>
@@ -38,15 +38,18 @@
 </t>
   </si>
   <si>
-    <t>card1</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
     <t>nama project</t>
   </si>
   <si>
+    <t>header</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pemberi Pekerjaan </t>
   </si>
   <si>
@@ -65,9 +68,6 @@
     <t>KL. 702/I/6/DO.1-2023, tanggal 04 Januari 2023</t>
   </si>
   <si>
-    <t>card2</t>
-  </si>
-  <si>
     <t>Nilai Pekerjaan</t>
   </si>
   <si>
@@ -86,9 +86,6 @@
     <t>Wilayah Daop I Jakarta</t>
   </si>
   <si>
-    <t>card3</t>
-  </si>
-  <si>
     <t>list</t>
   </si>
   <si>
@@ -96,21 +93,143 @@
   </si>
   <si>
     <t>Pengecekan Detail Komponen Jaringan LAA|Menstandarkan posisi kedudukan Hanger, ear, kedudukan pull off,trolley, messanger, kelengkapan Aksesories JLAA|Pengecatan Komponen Jaringan LAA &amp; Marking Hasil Pekerjaan yang sudah dilakukan Overhaul dengan Scotlight Reflektor</t>
+  </si>
+  <si>
+    <t>pendapatan</t>
+  </si>
+  <si>
+    <t>Nilai Kontrak (Rp)</t>
+  </si>
+  <si>
+    <t>615,761,483,126</t>
+  </si>
+  <si>
+    <t>Nilai DPP (Rp)</t>
+  </si>
+  <si>
+    <t>554,740,074,888</t>
+  </si>
+  <si>
+    <t>Target Pendapatan Akhir Bulan</t>
+  </si>
+  <si>
+    <t>17,550,784,846</t>
+  </si>
+  <si>
+    <t>penagihan</t>
+  </si>
+  <si>
+    <t>Proses Tagihan Belum Lengkap (Rp)</t>
+  </si>
+  <si>
+    <t>114,306,556,333</t>
+  </si>
+  <si>
+    <t>Proses Sudah Penerbiatan Invoice (Rp)</t>
+  </si>
+  <si>
+    <t>6,516,999,503</t>
+  </si>
+  <si>
+    <t>Total Tagihan (Rp)</t>
+  </si>
+  <si>
+    <t>120,823,555,836</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>Kumulatif Rencana</t>
+  </si>
+  <si>
+    <t>Kumulatif Realisasi</t>
+  </si>
+  <si>
+    <t>Kumulatif Deviasi</t>
+  </si>
+  <si>
+    <t>grafik_progress_bar</t>
+  </si>
+  <si>
+    <t>Realisasi</t>
+  </si>
+  <si>
+    <t>Rencana</t>
+  </si>
+  <si>
+    <t>list_float</t>
+  </si>
+  <si>
+    <t>grafik_line</t>
+  </si>
+  <si>
+    <t>1.5, 3.25, 4.75, 6.75, 8.75, 10.75, 13, 15.25, 17.5, 19.75, 22.25</t>
+  </si>
+  <si>
+    <t>0.24, 2.58, 5.24, 7.96, 11.4, 14.26, 16.92, 21.58, 25.45, 28.75, 33.78</t>
+  </si>
+  <si>
+    <t>pekerjaan_title</t>
+  </si>
+  <si>
+    <t>URAIAN KEGIATAN</t>
+  </si>
+  <si>
+    <t>PROGRES PEKERJAAN</t>
+  </si>
+  <si>
+    <t>pekerjaan_data</t>
+  </si>
+  <si>
+    <t>Pekerjaan Gelaran FO</t>
+  </si>
+  <si>
+    <t>Pembuatan dan pemasangan Patok Kabel FO</t>
+  </si>
+  <si>
+    <t>Pekerjaan Gelaran Kabel Persinyalan</t>
+  </si>
+  <si>
+    <t>Menyelesaikan penggelaran kabel persinyalan dari sinyal blok KAS arah SIG s.d titik EH PAP KAS</t>
+  </si>
+  <si>
+    <t>FAT EH Container</t>
+  </si>
+  <si>
+    <t>Baik dan dapat diterima</t>
+  </si>
+  <si>
+    <t>MOS EH Container</t>
+  </si>
+  <si>
+    <t>Baik dan dapat diterima 100%, dapat dibayarkan 75% selama belum terpasang dilapangan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.95"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -566,153 +685,165 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1084,16 +1215,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="9.765625" customWidth="1"/>
+    <col min="3" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="9.765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1109,7 +1240,7 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1121,13 +1252,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
         <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1138,13 +1269,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
         <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1155,13 +1286,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
         <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1169,15 +1300,15 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1186,15 +1317,15 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1203,15 +1334,15 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1223,14 +1354,329 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
       </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="3">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3">
+        <v>20.936</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5.265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="5:5">
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="5:5">
+      <c r="E29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>